<commit_message>
Finished rentals and equipment, only need to fix the rentals part then style
</commit_message>
<xml_diff>
--- a/cpsy200prototype/Services/data-samples.xlsx
+++ b/cpsy200prototype/Services/data-samples.xlsx
@@ -3,59 +3,114 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mryla\Documents\FBE\cpsy200prototype\cpsy200prototype\Services\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834EC89E-31EC-4CD3-AB77-59CEC1977EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="2040" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="645" yWindow="2040" windowWidth="21600" windowHeight="11235"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>rrrrrrre</t>
-  </si>
-  <si>
-    <t>eeeeeeeer</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>ererer@gmail.com</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>4321</t>
-  </si>
-  <si>
-    <t>Steve</t>
-  </si>
-  <si>
-    <t>0987654321</t>
-  </si>
-  <si>
-    <t>Stevesteve@gmail.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+  <si>
+    <t xml:space="preserve">1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rrrrrrre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eeeeeeeer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234567890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ererer@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0987654321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stevesteve@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4039013212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nile.grill@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shovel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dig dirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helmet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protects your head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pickaxe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dig Stuff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protects Head</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,11 +149,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -392,7 +447,7 @@
   <a:objectDefaults>
     <a:lnDef>
       <a:spPr/>
-      <a:bodyPr/>
+      <a:bodyPr rtlCol="0"/>
       <a:lstStyle/>
       <a:style>
         <a:lnRef idx="2">
@@ -420,11 +475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A2:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,45 +487,117 @@
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="11" max="11" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="H6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="H7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="H8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="0">
         <v>5</v>
       </c>
     </row>

</xml_diff>